<commit_message>
Slides Feitos, Planilha de Riscos Feita e Documentação Atualizada
</commit_message>
<xml_diff>
--- a/T.I/Divisão Sprints.xlsx
+++ b/T.I/Divisão Sprints.xlsx
@@ -75,7 +75,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +96,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,6 +126,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB2B2B2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -157,17 +170,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -177,6 +190,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3333"/>
+      <color rgb="FFFF5050"/>
       <color rgb="FFB2B2B2"/>
     </mruColors>
   </colors>
@@ -457,7 +472,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,10 +482,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="4"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -485,50 +500,50 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>